<commit_message>
fix parking tax bug
</commit_message>
<xml_diff>
--- a/COVID Budget Impact Analysis.xlsx
+++ b/COVID Budget Impact Analysis.xlsx
@@ -242,16 +242,16 @@
       <sz val="13"/>
     </font>
     <font>
+      <name val="Open Sans Regular"/>
+      <i val="1"/>
+      <color theme="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
       <name val="Calibri"/>
       <family val="2"/>
       <b val="1"/>
       <sz val="12"/>
-    </font>
-    <font>
-      <name val="Open Sans Regular"/>
-      <i val="1"/>
-      <color theme="1"/>
-      <sz val="10"/>
     </font>
     <font>
       <b val="1"/>
@@ -313,7 +313,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -625,6 +625,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -800,11 +815,6 @@
     <xf applyAlignment="1" borderId="14" fillId="0" fontId="22" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
     <xf applyAlignment="1" borderId="23" fillId="0" fontId="29" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -818,17 +828,32 @@
     <xf borderId="19" fillId="9" fontId="28" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="4"/>
     <xf borderId="0" fillId="0" fontId="28" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="4"/>
     <xf borderId="0" fillId="9" fontId="28" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf borderId="18" fillId="9" fontId="29" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="18" fillId="0" fontId="29" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="22" fillId="0" fontId="29" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="4"/>
+    <xf borderId="22" fillId="9" fontId="29" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="9" fontId="29" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="25" fillId="0" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="26" fillId="0" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="6" fillId="0" fontId="32" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="18" fillId="0" fontId="32" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="168" pivotButton="0" quotePrefix="0" xfId="4"/>
     <xf borderId="14" fillId="0" fontId="1" numFmtId="168" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf applyAlignment="1" borderId="27" fillId="0" fontId="32" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="28" fillId="0" fontId="33" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="27" fillId="0" fontId="32" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf applyAlignment="1" borderId="28" fillId="0" fontId="33" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="168" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf applyAlignment="1" borderId="23" fillId="0" fontId="29" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="27" fillId="0" fontId="29" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="25" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -876,17 +901,7 @@
     <xf applyAlignment="1" borderId="0" fillId="3" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="18" fillId="9" fontId="29" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="18" fillId="0" fontId="29" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="22" fillId="0" fontId="29" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf borderId="0" fillId="0" fontId="29" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf borderId="22" fillId="9" fontId="29" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="0" fillId="9" fontId="29" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="25" fillId="0" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="26" fillId="0" fontId="28" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="6" fillId="0" fontId="33" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="18" fillId="0" fontId="33" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="27" fillId="0" fontId="29" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="28" fillId="0" fontId="29" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="4" fontId="3" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="0">
@@ -898,10 +913,10 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="167" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="168" pivotButton="0" quotePrefix="0" xfId="4"/>
     <xf borderId="14" fillId="0" fontId="1" numFmtId="168" pivotButton="0" quotePrefix="0" xfId="4"/>
-    <xf applyAlignment="1" borderId="30" fillId="0" fontId="34" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="31" fillId="0" fontId="34" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="30" fillId="0" fontId="34" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf applyAlignment="1" borderId="31" fillId="0" fontId="34" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="168" pivotButton="0" quotePrefix="0" xfId="4"/>
@@ -1222,36 +1237,36 @@
   <dimension ref="B3:I19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0" zoomScale="110" zoomScaleNormal="110">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="85" width="7"/>
-    <col customWidth="1" max="2" min="2" style="85" width="31.5"/>
-    <col customWidth="1" max="5" min="3" style="85" width="12.83203125"/>
-    <col customWidth="1" max="6" min="6" style="85" width="0.6640625"/>
-    <col customWidth="1" max="9" min="7" style="85" width="12.83203125"/>
-    <col customWidth="1" max="13" min="10" style="85" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="14" style="85" width="10.83203125"/>
+    <col customWidth="1" max="1" min="1" style="82" width="7"/>
+    <col customWidth="1" max="2" min="2" style="82" width="31.5"/>
+    <col customWidth="1" max="5" min="3" style="82" width="12.83203125"/>
+    <col customWidth="1" max="6" min="6" style="82" width="0.6640625"/>
+    <col customWidth="1" max="9" min="7" style="82" width="12.83203125"/>
+    <col customWidth="1" max="15" min="10" style="82" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="16" style="82" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="20" r="3" s="111">
-      <c r="B3" s="104" t="inlineStr">
+    <row customHeight="1" ht="20" r="3" s="121">
+      <c r="B3" s="114" t="inlineStr">
         <is>
           <t>Estimated Tax Revenue Impacts for Major City of Philadelphia Taxes by Fiscal Year</t>
         </is>
       </c>
-      <c r="C3" s="105" t="n"/>
-      <c r="D3" s="105" t="n"/>
-      <c r="E3" s="105" t="n"/>
-      <c r="F3" s="105" t="n"/>
-      <c r="G3" s="105" t="n"/>
-      <c r="H3" s="105" t="n"/>
-      <c r="I3" s="106" t="n"/>
-    </row>
-    <row customHeight="1" ht="16" r="4" s="111">
-      <c r="B4" s="132" t="inlineStr">
+      <c r="C3" s="115" t="n"/>
+      <c r="D3" s="115" t="n"/>
+      <c r="E3" s="115" t="n"/>
+      <c r="F3" s="115" t="n"/>
+      <c r="G3" s="115" t="n"/>
+      <c r="H3" s="115" t="n"/>
+      <c r="I3" s="116" t="n"/>
+    </row>
+    <row customHeight="1" ht="16" r="4" s="121">
+      <c r="B4" s="101" t="inlineStr">
         <is>
           <t>Dollars in thousands</t>
         </is>
@@ -1260,17 +1275,17 @@
     </row>
     <row r="5">
       <c r="B5" s="58" t="n"/>
-      <c r="C5" s="107" t="inlineStr">
+      <c r="C5" s="117" t="inlineStr">
         <is>
           <t>Differences Relative to March Baseline</t>
         </is>
       </c>
-      <c r="D5" s="108" t="n"/>
-      <c r="E5" s="108" t="n"/>
-      <c r="F5" s="108" t="n"/>
-      <c r="G5" s="108" t="n"/>
-      <c r="H5" s="108" t="n"/>
-      <c r="I5" s="109" t="n"/>
+      <c r="D5" s="118" t="n"/>
+      <c r="E5" s="118" t="n"/>
+      <c r="F5" s="118" t="n"/>
+      <c r="G5" s="118" t="n"/>
+      <c r="H5" s="118" t="n"/>
+      <c r="I5" s="119" t="n"/>
     </row>
     <row r="6">
       <c r="B6" s="54" t="n"/>
@@ -1279,16 +1294,16 @@
           <t>Moderate</t>
         </is>
       </c>
-      <c r="D6" s="102" t="n"/>
-      <c r="E6" s="103" t="n"/>
+      <c r="D6" s="112" t="n"/>
+      <c r="E6" s="113" t="n"/>
       <c r="F6" s="59" t="n"/>
       <c r="G6" s="133" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
       </c>
-      <c r="H6" s="102" t="n"/>
-      <c r="I6" s="103" t="n"/>
+      <c r="H6" s="112" t="n"/>
+      <c r="I6" s="113" t="n"/>
     </row>
     <row r="7">
       <c r="B7" s="57" t="inlineStr">
@@ -1296,13 +1311,13 @@
           <t>Tax</t>
         </is>
       </c>
-      <c r="C7" s="84" t="n">
+      <c r="C7" s="81" t="n">
         <v>2020</v>
       </c>
-      <c r="D7" s="84" t="n">
+      <c r="D7" s="81" t="n">
         <v>2021</v>
       </c>
-      <c r="E7" s="84" t="inlineStr">
+      <c r="E7" s="81" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -1311,17 +1326,17 @@
       <c r="G7" s="56" t="n">
         <v>2020</v>
       </c>
-      <c r="H7" s="84" t="n">
+      <c r="H7" s="81" t="n">
         <v>2021</v>
       </c>
-      <c r="I7" s="84" t="inlineStr">
+      <c r="I7" s="81" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="88" t="inlineStr">
+      <c r="B8" s="85" t="inlineStr">
         <is>
           <t>Wage</t>
         </is>
@@ -1338,7 +1353,7 @@
         <f>SUM(C8:D8)</f>
         <v/>
       </c>
-      <c r="F8" s="92" t="n"/>
+      <c r="F8" s="89" t="n"/>
       <c r="G8" s="60">
         <f>Summary!G7/1000</f>
         <v/>
@@ -1353,7 +1368,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="89" t="inlineStr">
+      <c r="B9" s="86" t="inlineStr">
         <is>
           <t>Sales</t>
         </is>
@@ -1370,7 +1385,7 @@
         <f>SUM(C9:D9)</f>
         <v/>
       </c>
-      <c r="F9" s="93" t="n"/>
+      <c r="F9" s="90" t="n"/>
       <c r="G9" s="61">
         <f>Summary!G8/1000</f>
         <v/>
@@ -1385,7 +1400,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="90" t="inlineStr">
+      <c r="B10" s="87" t="inlineStr">
         <is>
           <t>Business Income and Receipts</t>
         </is>
@@ -1402,7 +1417,7 @@
         <f>SUM(C10:D10)</f>
         <v/>
       </c>
-      <c r="F10" s="94" t="n"/>
+      <c r="F10" s="91" t="n"/>
       <c r="G10" s="62">
         <f>Summary!G14/1000</f>
         <v/>
@@ -1417,7 +1432,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="89" t="inlineStr">
+      <c r="B11" s="86" t="inlineStr">
         <is>
           <t>Realty Transfer</t>
         </is>
@@ -1434,7 +1449,7 @@
         <f>SUM(C11:D11)</f>
         <v/>
       </c>
-      <c r="F11" s="93" t="n"/>
+      <c r="F11" s="90" t="n"/>
       <c r="G11" s="61">
         <f>Summary!G9/1000</f>
         <v/>
@@ -1449,7 +1464,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="90" t="inlineStr">
+      <c r="B12" s="87" t="inlineStr">
         <is>
           <t>Beverage</t>
         </is>
@@ -1466,7 +1481,7 @@
         <f>SUM(C12:D12)</f>
         <v/>
       </c>
-      <c r="F12" s="94" t="n"/>
+      <c r="F12" s="91" t="n"/>
       <c r="G12" s="62">
         <f>Summary!G10/1000</f>
         <v/>
@@ -1481,7 +1496,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="89" t="inlineStr">
+      <c r="B13" s="86" t="inlineStr">
         <is>
           <t>Amusement</t>
         </is>
@@ -1498,7 +1513,7 @@
         <f>SUM(C13:D13)</f>
         <v/>
       </c>
-      <c r="F13" s="93" t="n"/>
+      <c r="F13" s="90" t="n"/>
       <c r="G13" s="61">
         <f>Summary!G11/1000</f>
         <v/>
@@ -1513,7 +1528,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="90" t="inlineStr">
+      <c r="B14" s="87" t="inlineStr">
         <is>
           <t>Net Profits</t>
         </is>
@@ -1530,7 +1545,7 @@
         <f>SUM(C14:D14)</f>
         <v/>
       </c>
-      <c r="F14" s="94" t="n"/>
+      <c r="F14" s="91" t="n"/>
       <c r="G14" s="62">
         <f>Summary!G12/1000</f>
         <v/>
@@ -1545,7 +1560,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="89" t="inlineStr">
+      <c r="B15" s="86" t="inlineStr">
         <is>
           <t xml:space="preserve">Parking </t>
         </is>
@@ -1562,7 +1577,7 @@
         <f>SUM(C15:D15)</f>
         <v/>
       </c>
-      <c r="F15" s="93" t="n"/>
+      <c r="F15" s="90" t="n"/>
       <c r="G15" s="61">
         <f>Summary!G13/1000</f>
         <v/>
@@ -1577,112 +1592,111 @@
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="86" t="inlineStr">
+      <c r="B16" s="83" t="inlineStr">
         <is>
           <t>Total Difference</t>
         </is>
       </c>
-      <c r="C16" s="91">
+      <c r="C16" s="88">
         <f>SUM(C8:C15)</f>
         <v/>
       </c>
-      <c r="D16" s="91">
+      <c r="D16" s="88">
         <f>SUM(D8:D15)</f>
         <v/>
       </c>
-      <c r="E16" s="91">
+      <c r="E16" s="88">
         <f>SUM(C16:D16)</f>
         <v/>
       </c>
-      <c r="F16" s="87" t="n"/>
-      <c r="G16" s="91">
+      <c r="F16" s="84" t="n"/>
+      <c r="G16" s="88">
         <f>SUM(G8:G15)</f>
         <v/>
       </c>
-      <c r="H16" s="91">
+      <c r="H16" s="88">
         <f>SUM(H8:H15)</f>
         <v/>
       </c>
-      <c r="I16" s="91">
+      <c r="I16" s="88">
         <f>SUM(G16:H16)</f>
         <v/>
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="124" t="inlineStr">
+      <c r="B17" s="93" t="inlineStr">
         <is>
           <t>Baseline</t>
         </is>
       </c>
-      <c r="C17" s="125" t="n">
-        <v>3726400</v>
-      </c>
-      <c r="D17" s="125" t="n">
-        <v>3860800</v>
-      </c>
-      <c r="E17" s="125">
+      <c r="C17" s="94" t="n">
+        <v>3726419</v>
+      </c>
+      <c r="D17" s="94" t="n">
+        <v>3860761</v>
+      </c>
+      <c r="E17" s="94">
         <f>C17+D17</f>
         <v/>
       </c>
-      <c r="F17" s="126" t="n"/>
-      <c r="G17" s="125">
-        <f>C17</f>
-        <v/>
-      </c>
-      <c r="H17" s="125">
+      <c r="F17" s="95" t="n"/>
+      <c r="G17" s="94" t="n">
+        <v>3726419</v>
+      </c>
+      <c r="H17" s="94">
         <f>D17</f>
         <v/>
       </c>
-      <c r="I17" s="125">
+      <c r="I17" s="94">
         <f>E17</f>
         <v/>
       </c>
     </row>
     <row r="18">
-      <c r="B18" s="123" t="inlineStr">
+      <c r="B18" s="92" t="inlineStr">
         <is>
           <t>Percent Change from Baseline</t>
         </is>
       </c>
-      <c r="C18" s="127">
+      <c r="C18" s="96">
         <f>C16/C17</f>
         <v/>
       </c>
-      <c r="D18" s="127">
+      <c r="D18" s="96">
         <f>D16/D17</f>
         <v/>
       </c>
-      <c r="E18" s="127">
+      <c r="E18" s="96">
         <f>E16/E17</f>
         <v/>
       </c>
-      <c r="F18" s="128" t="n"/>
-      <c r="G18" s="127">
+      <c r="F18" s="97" t="n"/>
+      <c r="G18" s="96">
         <f>G16/G17</f>
         <v/>
       </c>
-      <c r="H18" s="127">
+      <c r="H18" s="96">
         <f>H16/H17</f>
         <v/>
       </c>
-      <c r="I18" s="127">
+      <c r="I18" s="96">
         <f>I16/I17</f>
         <v/>
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="131" t="inlineStr">
+      <c r="B19" s="100" t="inlineStr">
         <is>
           <t>Note: Baseline estimates from FY21 - FY25 Five Year Financial Plan, as proposed on March 5, 2020.</t>
         </is>
       </c>
-      <c r="C19" s="129" t="n"/>
-      <c r="D19" s="129" t="n"/>
-      <c r="E19" s="129" t="n"/>
-      <c r="F19" s="129" t="n"/>
-      <c r="G19" s="129" t="n"/>
-      <c r="H19" s="129" t="n"/>
-      <c r="I19" s="130" t="n"/>
+      <c r="C19" s="98" t="n"/>
+      <c r="D19" s="98" t="n"/>
+      <c r="E19" s="98" t="n"/>
+      <c r="F19" s="98" t="n"/>
+      <c r="G19" s="98" t="n"/>
+      <c r="H19" s="98" t="n"/>
+      <c r="I19" s="99" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1711,24 +1725,24 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="117" width="15.1640625"/>
-    <col customWidth="1" max="2" min="2" style="117" width="16"/>
-    <col bestFit="1" customWidth="1" max="10" min="3" style="117" width="15"/>
-    <col bestFit="1" customWidth="1" max="12" min="11" style="117" width="16"/>
-    <col bestFit="1" customWidth="1" max="22" min="13" style="117" width="15"/>
-    <col customWidth="1" max="54" min="23" style="117" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="55" style="117" width="10.83203125"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="127" width="15.1640625"/>
+    <col customWidth="1" max="2" min="2" style="127" width="16"/>
+    <col bestFit="1" customWidth="1" max="10" min="3" style="127" width="15"/>
+    <col bestFit="1" customWidth="1" max="12" min="11" style="127" width="16"/>
+    <col bestFit="1" customWidth="1" max="22" min="13" style="127" width="15"/>
+    <col customWidth="1" max="56" min="23" style="127" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="57" style="127" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="26" r="1" s="111">
-      <c r="A1" s="116" t="inlineStr">
+    <row customHeight="1" ht="26" r="1" s="121">
+      <c r="A1" s="126" t="inlineStr">
         <is>
           <t>Amusement Tax Forecasts</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="3" s="111" thickBot="1"/>
-    <row customHeight="1" ht="19" r="4" s="111" thickBot="1">
+    <row customHeight="1" ht="17" r="3" s="121" thickBot="1"/>
+    <row customHeight="1" ht="19" r="4" s="121" thickBot="1">
       <c r="B4" s="4" t="n"/>
       <c r="D4" s="18" t="n"/>
       <c r="E4" s="23" t="inlineStr">
@@ -1742,7 +1756,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="5" s="111">
+    <row customHeight="1" ht="19" r="5" s="121">
       <c r="B5" s="4" t="n"/>
       <c r="D5" s="19" t="inlineStr">
         <is>
@@ -1758,7 +1772,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="6" s="111">
+    <row customHeight="1" ht="19" r="6" s="121">
       <c r="B6" s="4" t="n"/>
       <c r="D6" s="20" t="inlineStr">
         <is>
@@ -1774,7 +1788,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="7" s="111" thickBot="1">
+    <row customHeight="1" ht="21" r="7" s="121" thickBot="1">
       <c r="D7" s="21" t="inlineStr">
         <is>
           <t>FY22</t>
@@ -1790,7 +1804,7 @@
       </c>
       <c r="J7" s="32" t="n"/>
     </row>
-    <row customHeight="1" ht="20" r="8" s="111" thickBot="1" thickTop="1">
+    <row customHeight="1" ht="20" r="8" s="121" thickBot="1" thickTop="1">
       <c r="B8" s="11" t="n"/>
       <c r="D8" s="22" t="inlineStr">
         <is>
@@ -1806,11 +1820,11 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="20" r="9" s="111">
+    <row customHeight="1" ht="20" r="9" s="121">
       <c r="B9" s="12" t="n"/>
     </row>
-    <row customHeight="1" ht="26" r="11" s="111">
-      <c r="A11" s="118" t="inlineStr">
+    <row customHeight="1" ht="26" r="11" s="121">
+      <c r="A11" s="128" t="inlineStr">
         <is>
           <t>Moderate Scenario</t>
         </is>
@@ -1829,35 +1843,35 @@
       <c r="V11" s="30" t="n"/>
     </row>
     <row r="14">
-      <c r="B14" s="121" t="inlineStr">
+      <c r="B14" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2020</t>
         </is>
       </c>
-      <c r="C14" s="108" t="n"/>
-      <c r="D14" s="108" t="n"/>
-      <c r="E14" s="108" t="n"/>
-      <c r="F14" s="108" t="n"/>
-      <c r="G14" s="108" t="n"/>
-      <c r="H14" s="108" t="n"/>
-      <c r="I14" s="108" t="n"/>
-      <c r="J14" s="109" t="n"/>
-      <c r="K14" s="121" t="inlineStr">
+      <c r="C14" s="118" t="n"/>
+      <c r="D14" s="118" t="n"/>
+      <c r="E14" s="118" t="n"/>
+      <c r="F14" s="118" t="n"/>
+      <c r="G14" s="118" t="n"/>
+      <c r="H14" s="118" t="n"/>
+      <c r="I14" s="118" t="n"/>
+      <c r="J14" s="119" t="n"/>
+      <c r="K14" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2021</t>
         </is>
       </c>
-      <c r="L14" s="108" t="n"/>
-      <c r="M14" s="108" t="n"/>
-      <c r="N14" s="108" t="n"/>
-      <c r="O14" s="108" t="n"/>
-      <c r="P14" s="108" t="n"/>
-      <c r="Q14" s="108" t="n"/>
-      <c r="R14" s="108" t="n"/>
-      <c r="S14" s="108" t="n"/>
-      <c r="T14" s="108" t="n"/>
-      <c r="U14" s="108" t="n"/>
-      <c r="V14" s="109" t="n"/>
+      <c r="L14" s="118" t="n"/>
+      <c r="M14" s="118" t="n"/>
+      <c r="N14" s="118" t="n"/>
+      <c r="O14" s="118" t="n"/>
+      <c r="P14" s="118" t="n"/>
+      <c r="Q14" s="118" t="n"/>
+      <c r="R14" s="118" t="n"/>
+      <c r="S14" s="118" t="n"/>
+      <c r="T14" s="118" t="n"/>
+      <c r="U14" s="118" t="n"/>
+      <c r="V14" s="119" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="n"/>
@@ -2131,8 +2145,8 @@
       <c r="I19" s="73" t="n"/>
       <c r="J19" s="73" t="n"/>
     </row>
-    <row customHeight="1" ht="26" r="20" s="111">
-      <c r="A20" s="118" t="inlineStr">
+    <row customHeight="1" ht="26" r="20" s="121">
+      <c r="A20" s="128" t="inlineStr">
         <is>
           <t>Severe Scenario</t>
         </is>
@@ -2151,35 +2165,35 @@
       <c r="V20" s="30" t="n"/>
     </row>
     <row r="23">
-      <c r="B23" s="121" t="inlineStr">
+      <c r="B23" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2020</t>
         </is>
       </c>
-      <c r="C23" s="108" t="n"/>
-      <c r="D23" s="108" t="n"/>
-      <c r="E23" s="108" t="n"/>
-      <c r="F23" s="108" t="n"/>
-      <c r="G23" s="108" t="n"/>
-      <c r="H23" s="108" t="n"/>
-      <c r="I23" s="108" t="n"/>
-      <c r="J23" s="109" t="n"/>
-      <c r="K23" s="121" t="inlineStr">
+      <c r="C23" s="118" t="n"/>
+      <c r="D23" s="118" t="n"/>
+      <c r="E23" s="118" t="n"/>
+      <c r="F23" s="118" t="n"/>
+      <c r="G23" s="118" t="n"/>
+      <c r="H23" s="118" t="n"/>
+      <c r="I23" s="118" t="n"/>
+      <c r="J23" s="119" t="n"/>
+      <c r="K23" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2021</t>
         </is>
       </c>
-      <c r="L23" s="108" t="n"/>
-      <c r="M23" s="108" t="n"/>
-      <c r="N23" s="108" t="n"/>
-      <c r="O23" s="108" t="n"/>
-      <c r="P23" s="108" t="n"/>
-      <c r="Q23" s="108" t="n"/>
-      <c r="R23" s="108" t="n"/>
-      <c r="S23" s="108" t="n"/>
-      <c r="T23" s="108" t="n"/>
-      <c r="U23" s="108" t="n"/>
-      <c r="V23" s="109" t="n"/>
+      <c r="L23" s="118" t="n"/>
+      <c r="M23" s="118" t="n"/>
+      <c r="N23" s="118" t="n"/>
+      <c r="O23" s="118" t="n"/>
+      <c r="P23" s="118" t="n"/>
+      <c r="Q23" s="118" t="n"/>
+      <c r="R23" s="118" t="n"/>
+      <c r="S23" s="118" t="n"/>
+      <c r="T23" s="118" t="n"/>
+      <c r="U23" s="118" t="n"/>
+      <c r="V23" s="119" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="n"/>
@@ -2429,8 +2443,8 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="26" r="30" s="111">
-      <c r="A30" s="122" t="inlineStr">
+    <row customHeight="1" ht="26" r="30" s="121">
+      <c r="A30" s="132" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
@@ -2758,24 +2772,24 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="117" width="15.1640625"/>
-    <col customWidth="1" max="2" min="2" style="117" width="16"/>
-    <col bestFit="1" customWidth="1" max="10" min="3" style="117" width="15"/>
-    <col bestFit="1" customWidth="1" max="12" min="11" style="117" width="16"/>
-    <col bestFit="1" customWidth="1" max="22" min="13" style="117" width="15"/>
-    <col customWidth="1" max="54" min="23" style="117" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="55" style="117" width="10.83203125"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="127" width="15.1640625"/>
+    <col customWidth="1" max="2" min="2" style="127" width="16"/>
+    <col bestFit="1" customWidth="1" max="10" min="3" style="127" width="15"/>
+    <col bestFit="1" customWidth="1" max="12" min="11" style="127" width="16"/>
+    <col bestFit="1" customWidth="1" max="22" min="13" style="127" width="15"/>
+    <col customWidth="1" max="56" min="23" style="127" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="57" style="127" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="26" r="1" s="111">
-      <c r="A1" s="116" t="inlineStr">
+    <row customHeight="1" ht="26" r="1" s="121">
+      <c r="A1" s="126" t="inlineStr">
         <is>
           <t>NPT Forecasts</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="3" s="111" thickBot="1"/>
-    <row customHeight="1" ht="19" r="4" s="111" thickBot="1">
+    <row customHeight="1" ht="17" r="3" s="121" thickBot="1"/>
+    <row customHeight="1" ht="19" r="4" s="121" thickBot="1">
       <c r="B4" s="4" t="n"/>
       <c r="D4" s="18" t="n"/>
       <c r="E4" s="23" t="inlineStr">
@@ -2789,7 +2803,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="5" s="111">
+    <row customHeight="1" ht="19" r="5" s="121">
       <c r="B5" s="4" t="n"/>
       <c r="D5" s="19" t="inlineStr">
         <is>
@@ -2805,7 +2819,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="6" s="111">
+    <row customHeight="1" ht="19" r="6" s="121">
       <c r="B6" s="4" t="n"/>
       <c r="D6" s="20" t="inlineStr">
         <is>
@@ -2821,7 +2835,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="7" s="111" thickBot="1">
+    <row customHeight="1" ht="21" r="7" s="121" thickBot="1">
       <c r="D7" s="21" t="inlineStr">
         <is>
           <t>FY22</t>
@@ -2837,7 +2851,7 @@
       </c>
       <c r="J7" s="32" t="n"/>
     </row>
-    <row customHeight="1" ht="20" r="8" s="111" thickBot="1" thickTop="1">
+    <row customHeight="1" ht="20" r="8" s="121" thickBot="1" thickTop="1">
       <c r="B8" s="11" t="n"/>
       <c r="D8" s="22" t="inlineStr">
         <is>
@@ -2853,11 +2867,11 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="20" r="9" s="111">
+    <row customHeight="1" ht="20" r="9" s="121">
       <c r="B9" s="12" t="n"/>
     </row>
-    <row customHeight="1" ht="26" r="11" s="111">
-      <c r="A11" s="118" t="inlineStr">
+    <row customHeight="1" ht="26" r="11" s="121">
+      <c r="A11" s="128" t="inlineStr">
         <is>
           <t>Moderate Scenario</t>
         </is>
@@ -2876,35 +2890,35 @@
       <c r="V11" s="30" t="n"/>
     </row>
     <row r="14">
-      <c r="B14" s="121" t="inlineStr">
+      <c r="B14" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2020</t>
         </is>
       </c>
-      <c r="C14" s="108" t="n"/>
-      <c r="D14" s="108" t="n"/>
-      <c r="E14" s="108" t="n"/>
-      <c r="F14" s="108" t="n"/>
-      <c r="G14" s="108" t="n"/>
-      <c r="H14" s="108" t="n"/>
-      <c r="I14" s="108" t="n"/>
-      <c r="J14" s="109" t="n"/>
-      <c r="K14" s="121" t="inlineStr">
+      <c r="C14" s="118" t="n"/>
+      <c r="D14" s="118" t="n"/>
+      <c r="E14" s="118" t="n"/>
+      <c r="F14" s="118" t="n"/>
+      <c r="G14" s="118" t="n"/>
+      <c r="H14" s="118" t="n"/>
+      <c r="I14" s="118" t="n"/>
+      <c r="J14" s="119" t="n"/>
+      <c r="K14" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2021</t>
         </is>
       </c>
-      <c r="L14" s="108" t="n"/>
-      <c r="M14" s="108" t="n"/>
-      <c r="N14" s="108" t="n"/>
-      <c r="O14" s="108" t="n"/>
-      <c r="P14" s="108" t="n"/>
-      <c r="Q14" s="108" t="n"/>
-      <c r="R14" s="108" t="n"/>
-      <c r="S14" s="108" t="n"/>
-      <c r="T14" s="108" t="n"/>
-      <c r="U14" s="108" t="n"/>
-      <c r="V14" s="109" t="n"/>
+      <c r="L14" s="118" t="n"/>
+      <c r="M14" s="118" t="n"/>
+      <c r="N14" s="118" t="n"/>
+      <c r="O14" s="118" t="n"/>
+      <c r="P14" s="118" t="n"/>
+      <c r="Q14" s="118" t="n"/>
+      <c r="R14" s="118" t="n"/>
+      <c r="S14" s="118" t="n"/>
+      <c r="T14" s="118" t="n"/>
+      <c r="U14" s="118" t="n"/>
+      <c r="V14" s="119" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="n"/>
@@ -3178,8 +3192,8 @@
       <c r="I19" s="73" t="n"/>
       <c r="J19" s="73" t="n"/>
     </row>
-    <row customHeight="1" ht="26" r="20" s="111">
-      <c r="A20" s="118" t="inlineStr">
+    <row customHeight="1" ht="26" r="20" s="121">
+      <c r="A20" s="128" t="inlineStr">
         <is>
           <t>Severe Scenario</t>
         </is>
@@ -3198,35 +3212,35 @@
       <c r="V20" s="30" t="n"/>
     </row>
     <row r="23">
-      <c r="B23" s="121" t="inlineStr">
+      <c r="B23" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2020</t>
         </is>
       </c>
-      <c r="C23" s="108" t="n"/>
-      <c r="D23" s="108" t="n"/>
-      <c r="E23" s="108" t="n"/>
-      <c r="F23" s="108" t="n"/>
-      <c r="G23" s="108" t="n"/>
-      <c r="H23" s="108" t="n"/>
-      <c r="I23" s="108" t="n"/>
-      <c r="J23" s="109" t="n"/>
-      <c r="K23" s="121" t="inlineStr">
+      <c r="C23" s="118" t="n"/>
+      <c r="D23" s="118" t="n"/>
+      <c r="E23" s="118" t="n"/>
+      <c r="F23" s="118" t="n"/>
+      <c r="G23" s="118" t="n"/>
+      <c r="H23" s="118" t="n"/>
+      <c r="I23" s="118" t="n"/>
+      <c r="J23" s="119" t="n"/>
+      <c r="K23" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2021</t>
         </is>
       </c>
-      <c r="L23" s="108" t="n"/>
-      <c r="M23" s="108" t="n"/>
-      <c r="N23" s="108" t="n"/>
-      <c r="O23" s="108" t="n"/>
-      <c r="P23" s="108" t="n"/>
-      <c r="Q23" s="108" t="n"/>
-      <c r="R23" s="108" t="n"/>
-      <c r="S23" s="108" t="n"/>
-      <c r="T23" s="108" t="n"/>
-      <c r="U23" s="108" t="n"/>
-      <c r="V23" s="109" t="n"/>
+      <c r="L23" s="118" t="n"/>
+      <c r="M23" s="118" t="n"/>
+      <c r="N23" s="118" t="n"/>
+      <c r="O23" s="118" t="n"/>
+      <c r="P23" s="118" t="n"/>
+      <c r="Q23" s="118" t="n"/>
+      <c r="R23" s="118" t="n"/>
+      <c r="S23" s="118" t="n"/>
+      <c r="T23" s="118" t="n"/>
+      <c r="U23" s="118" t="n"/>
+      <c r="V23" s="119" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="n"/>
@@ -3476,8 +3490,8 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="26" r="30" s="111">
-      <c r="A30" s="122" t="inlineStr">
+    <row customHeight="1" ht="26" r="30" s="121">
+      <c r="A30" s="132" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
@@ -3799,22 +3813,22 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="115" zoomScaleNormal="125" zoomScalePageLayoutView="125">
-      <selection activeCell="A7" sqref="A7:A14"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="111" width="35.83203125"/>
-    <col bestFit="1" customWidth="1" max="4" min="2" style="111" width="13.6640625"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="111" width="12.5"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="111" width="35.5"/>
-    <col bestFit="1" customWidth="1" max="9" min="7" style="111" width="13.6640625"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="111" width="12.33203125"/>
-    <col customWidth="1" max="45" min="11" style="111" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="46" style="111" width="10.83203125"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="121" width="35.83203125"/>
+    <col bestFit="1" customWidth="1" max="4" min="2" style="121" width="13.6640625"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="121" width="12.5"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" style="121" width="35.5"/>
+    <col bestFit="1" customWidth="1" max="9" min="7" style="121" width="13.6640625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="121" width="12.33203125"/>
+    <col customWidth="1" max="47" min="11" style="121" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="48" style="121" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="21" r="1" s="111">
+    <row customHeight="1" ht="21" r="1" s="121">
       <c r="A1" s="134" t="inlineStr">
         <is>
           <t>Moderate</t>
@@ -3864,7 +3878,7 @@
         </is>
       </c>
     </row>
-    <row hidden="1" r="4" s="111">
+    <row hidden="1" r="4" s="121">
       <c r="A4" s="31" t="inlineStr">
         <is>
           <t>Estimated Fund Balance pre-COVID</t>
@@ -3887,7 +3901,7 @@
       <c r="H4" s="51" t="n"/>
       <c r="I4" s="51" t="n"/>
     </row>
-    <row hidden="1" r="5" s="111">
+    <row hidden="1" r="5" s="121">
       <c r="A5" s="31" t="n"/>
       <c r="B5" s="51" t="n"/>
       <c r="C5" s="51" t="n"/>
@@ -4166,7 +4180,7 @@
         </is>
       </c>
       <c r="G13" s="51">
-        <f>'Parking Scenario Analysis'!E5</f>
+        <f>'Parking Scenario Analysis'!F5</f>
         <v/>
       </c>
       <c r="H13" s="51">
@@ -4179,7 +4193,7 @@
       </c>
       <c r="J13" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="14" s="111" thickBot="1">
+    <row customHeight="1" ht="17" r="14" s="121" thickBot="1">
       <c r="A14" s="27" t="inlineStr">
         <is>
           <t>BIRT</t>
@@ -4217,7 +4231,7 @@
       </c>
       <c r="J14" s="3" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="15" s="111" thickTop="1">
+    <row customHeight="1" ht="17" r="15" s="121" thickTop="1">
       <c r="A15" s="1" t="inlineStr">
         <is>
           <t>Total</t>
@@ -4293,7 +4307,7 @@
       <c r="H19" s="51" t="n"/>
       <c r="I19" s="51" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="20" s="111">
+    <row customHeight="1" ht="17" r="20" s="121">
       <c r="B20" s="51" t="n"/>
       <c r="C20" s="51" t="n"/>
       <c r="D20" s="51" t="n"/>
@@ -4302,7 +4316,7 @@
       <c r="H20" s="51" t="n"/>
       <c r="I20" s="51" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="21" s="111">
+    <row customHeight="1" ht="17" r="21" s="121">
       <c r="A21" s="52" t="n"/>
       <c r="B21" s="53" t="n"/>
       <c r="C21" s="53" t="n"/>
@@ -4412,26 +4426,26 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="111" width="48.83203125"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="114" width="8"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="111" width="8.83203125"/>
-    <col bestFit="1" customWidth="1" max="9" min="4" style="111" width="8"/>
-    <col customWidth="1" max="10" min="10" style="111" width="10.83203125"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="111" width="48.83203125"/>
-    <col bestFit="1" customWidth="1" max="12" min="12" style="111" width="8"/>
-    <col bestFit="1" customWidth="1" max="13" min="13" style="111" width="8.83203125"/>
-    <col bestFit="1" customWidth="1" max="19" min="14" style="111" width="8"/>
-    <col customWidth="1" max="30" min="20" style="111" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="31" style="111" width="10.83203125"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="121" width="48.83203125"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="124" width="8"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="121" width="8.83203125"/>
+    <col bestFit="1" customWidth="1" max="9" min="4" style="121" width="8"/>
+    <col customWidth="1" max="10" min="10" style="121" width="10.83203125"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" style="121" width="48.83203125"/>
+    <col bestFit="1" customWidth="1" max="12" min="12" style="121" width="8"/>
+    <col bestFit="1" customWidth="1" max="13" min="13" style="121" width="8.83203125"/>
+    <col bestFit="1" customWidth="1" max="19" min="14" style="121" width="8"/>
+    <col customWidth="1" max="32" min="20" style="121" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="33" style="121" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="26" r="1" s="111">
-      <c r="A1" s="113" t="inlineStr">
+    <row customHeight="1" ht="26" r="1" s="121">
+      <c r="A1" s="123" t="inlineStr">
         <is>
           <t>Moderate</t>
         </is>
       </c>
-      <c r="K1" s="115" t="inlineStr">
+      <c r="K1" s="125" t="inlineStr">
         <is>
           <t>Severe</t>
         </is>
@@ -4439,11 +4453,11 @@
     </row>
     <row r="2">
       <c r="A2" s="43" t="n"/>
-      <c r="C2" s="114" t="n"/>
-      <c r="D2" s="114" t="n"/>
-      <c r="G2" s="114" t="n"/>
-      <c r="H2" s="114" t="n"/>
-      <c r="I2" s="114" t="n"/>
+      <c r="C2" s="124" t="n"/>
+      <c r="D2" s="124" t="n"/>
+      <c r="G2" s="124" t="n"/>
+      <c r="H2" s="124" t="n"/>
+      <c r="I2" s="124" t="n"/>
       <c r="K2" s="43" t="n"/>
     </row>
     <row r="3">
@@ -4452,7 +4466,7 @@
       <c r="K3" s="43" t="n"/>
       <c r="S3" s="43" t="n"/>
     </row>
-    <row customHeight="1" ht="20" r="4" s="111">
+    <row customHeight="1" ht="20" r="4" s="121">
       <c r="A4" s="36" t="inlineStr">
         <is>
           <t>Wage</t>
@@ -5887,7 +5901,7 @@
       <c r="K31" s="39" t="n"/>
       <c r="L31" s="43" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="32" s="111">
+    <row customHeight="1" ht="21" r="32" s="121">
       <c r="A32" s="36" t="inlineStr">
         <is>
           <t>Sales</t>
@@ -6798,7 +6812,7 @@
       <c r="R51" s="43" t="n"/>
       <c r="S51" s="43" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="52" s="111">
+    <row customHeight="1" ht="21" r="52" s="121">
       <c r="A52" s="49" t="inlineStr">
         <is>
           <t>RTT</t>
@@ -6975,7 +6989,7 @@
       <c r="K56" s="39" t="n"/>
       <c r="L56" s="43" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="57" s="111">
+    <row customHeight="1" ht="21" r="57" s="121">
       <c r="A57" s="49" t="inlineStr">
         <is>
           <t>BIRT</t>
@@ -8264,7 +8278,7 @@
       <c r="A83" s="39" t="n"/>
       <c r="K83" s="39" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="84" s="111">
+    <row customHeight="1" ht="21" r="84" s="121">
       <c r="A84" s="49" t="inlineStr">
         <is>
           <t>Soda</t>
@@ -8426,7 +8440,7 @@
       <c r="K89" s="39" t="n"/>
       <c r="L89" s="43" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="90" s="111">
+    <row customHeight="1" ht="21" r="90" s="121">
       <c r="A90" s="49" t="inlineStr">
         <is>
           <t>Parking</t>
@@ -8586,7 +8600,7 @@
       <c r="K95" s="39" t="n"/>
       <c r="L95" s="43" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="96" s="111">
+    <row customHeight="1" ht="21" r="96" s="121">
       <c r="A96" s="49" t="inlineStr">
         <is>
           <t>Amusement</t>
@@ -8746,7 +8760,7 @@
       <c r="K101" s="43" t="n"/>
       <c r="L101" s="43" t="n"/>
     </row>
-    <row customHeight="1" ht="21" r="102" s="111">
+    <row customHeight="1" ht="21" r="102" s="121">
       <c r="A102" s="49" t="inlineStr">
         <is>
           <t>NPT</t>
@@ -9519,26 +9533,26 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="117" width="21.6640625"/>
-    <col customWidth="1" max="2" min="2" style="117" width="16.5"/>
-    <col bestFit="1" customWidth="1" max="11" min="3" style="117" width="16"/>
-    <col customWidth="1" max="12" min="12" style="117" width="18.1640625"/>
-    <col bestFit="1" customWidth="1" max="23" min="13" style="117" width="16"/>
-    <col customWidth="1" max="49" min="24" style="117" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="50" style="117" width="10.83203125"/>
+    <col customWidth="1" max="1" min="1" style="127" width="21.6640625"/>
+    <col customWidth="1" max="2" min="2" style="127" width="16.5"/>
+    <col bestFit="1" customWidth="1" max="11" min="3" style="127" width="16"/>
+    <col customWidth="1" max="12" min="12" style="127" width="18.1640625"/>
+    <col bestFit="1" customWidth="1" max="23" min="13" style="127" width="16"/>
+    <col customWidth="1" max="51" min="24" style="127" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="52" style="127" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="26" r="1" s="111">
-      <c r="A1" s="116" t="inlineStr">
+    <row customHeight="1" ht="26" r="1" s="121">
+      <c r="A1" s="126" t="inlineStr">
         <is>
           <t>Wage Tax Forecasts</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="3" s="111" thickBot="1">
+    <row customHeight="1" ht="19" r="3" s="121" thickBot="1">
       <c r="B3" s="4" t="n"/>
     </row>
-    <row customHeight="1" ht="19" r="4" s="111" thickBot="1">
+    <row customHeight="1" ht="19" r="4" s="121" thickBot="1">
       <c r="B4" s="4" t="n"/>
       <c r="D4" s="18" t="n"/>
       <c r="E4" s="23" t="inlineStr">
@@ -9552,7 +9566,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="5" s="111">
+    <row customHeight="1" ht="19" r="5" s="121">
       <c r="B5" s="4" t="n"/>
       <c r="D5" s="19" t="inlineStr">
         <is>
@@ -9568,7 +9582,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="6" s="111">
+    <row customHeight="1" ht="19" r="6" s="121">
       <c r="B6" s="4" t="n"/>
       <c r="D6" s="20" t="inlineStr">
         <is>
@@ -9587,7 +9601,7 @@
       <c r="L6" s="32" t="n"/>
       <c r="M6" s="32" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="7" s="111" thickBot="1">
+    <row customHeight="1" ht="17" r="7" s="121" thickBot="1">
       <c r="D7" s="21" t="inlineStr">
         <is>
           <t>FY22</t>
@@ -9602,7 +9616,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="20" r="8" s="111" thickBot="1" thickTop="1">
+    <row customHeight="1" ht="20" r="8" s="121" thickBot="1" thickTop="1">
       <c r="D8" s="22" t="inlineStr">
         <is>
           <t>Total</t>
@@ -9617,12 +9631,12 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="9" s="111">
+    <row customHeight="1" ht="19" r="9" s="121">
       <c r="B9" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="10" s="111"/>
-    <row customHeight="1" ht="26" r="11" s="111">
-      <c r="A11" s="118" t="inlineStr">
+    <row customHeight="1" ht="17" r="10" s="121"/>
+    <row customHeight="1" ht="26" r="11" s="121">
+      <c r="A11" s="128" t="inlineStr">
         <is>
           <t>Moderate Duration Scenario</t>
         </is>
@@ -9646,7 +9660,7 @@
     <row r="13">
       <c r="M13" s="71" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="14" s="111">
+    <row customHeight="1" ht="17" r="14" s="121">
       <c r="M14" s="71" t="n"/>
     </row>
     <row r="15">
@@ -11626,7 +11640,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="37" s="111" thickBot="1">
+    <row customHeight="1" ht="17" r="37" s="121" thickBot="1">
       <c r="A37" s="33" t="inlineStr">
         <is>
           <t>Wholesale Trade</t>
@@ -11717,7 +11731,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="38" s="111" thickTop="1">
+    <row customHeight="1" ht="16" r="38" s="121" thickTop="1">
       <c r="A38" s="7" t="inlineStr">
         <is>
           <t>Total</t>
@@ -11911,7 +11925,7 @@
       <c r="I40" s="73" t="n"/>
       <c r="J40" s="73" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="41" s="111">
+    <row customHeight="1" ht="17" r="41" s="121">
       <c r="A41" s="7" t="n"/>
       <c r="B41" s="73" t="n"/>
       <c r="C41" s="73" t="n"/>
@@ -11923,8 +11937,8 @@
       <c r="I41" s="73" t="n"/>
       <c r="J41" s="73" t="n"/>
     </row>
-    <row customHeight="1" ht="26" r="42" s="111">
-      <c r="A42" s="118" t="inlineStr">
+    <row customHeight="1" ht="26" r="42" s="121">
+      <c r="A42" s="128" t="inlineStr">
         <is>
           <t>Severe Duration Scenario</t>
         </is>
@@ -11948,7 +11962,7 @@
     <row r="44">
       <c r="M44" s="71" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="45" s="111">
+    <row customHeight="1" ht="17" r="45" s="121">
       <c r="M45" s="71" t="n"/>
     </row>
     <row r="46">
@@ -13018,7 +13032,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="58" s="111">
+    <row customHeight="1" ht="16" r="58" s="121">
       <c r="A58" s="2" t="inlineStr">
         <is>
           <t>Public Utilities</t>
@@ -13109,7 +13123,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="59" s="111">
+    <row customHeight="1" ht="16" r="59" s="121">
       <c r="A59" s="2" t="inlineStr">
         <is>
           <t>Publishing, Broadcasting, and Other Information</t>
@@ -13200,7 +13214,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="60" s="111">
+    <row customHeight="1" ht="16" r="60" s="121">
       <c r="A60" s="2" t="inlineStr">
         <is>
           <t>Real Estate, Rental and Leasing</t>
@@ -13291,7 +13305,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="61" s="111">
+    <row customHeight="1" ht="16" r="61" s="121">
       <c r="A61" s="2" t="inlineStr">
         <is>
           <t>Restaurants</t>
@@ -13382,7 +13396,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="62" s="111">
+    <row customHeight="1" ht="16" r="62" s="121">
       <c r="A62" s="2" t="inlineStr">
         <is>
           <t>Retail Trade</t>
@@ -13473,7 +13487,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="63" s="111">
+    <row customHeight="1" ht="16" r="63" s="121">
       <c r="A63" s="2" t="inlineStr">
         <is>
           <t>Securities / Financial Investments</t>
@@ -13564,7 +13578,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="64" s="111">
+    <row customHeight="1" ht="16" r="64" s="121">
       <c r="A64" s="2" t="inlineStr">
         <is>
           <t>Sport Teams</t>
@@ -13655,7 +13669,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="65" s="111">
+    <row customHeight="1" ht="16" r="65" s="121">
       <c r="A65" s="2" t="inlineStr">
         <is>
           <t>Telecommunication</t>
@@ -13746,7 +13760,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="66" s="111">
+    <row customHeight="1" ht="16" r="66" s="121">
       <c r="A66" s="2" t="inlineStr">
         <is>
           <t>Transportation and Warehousing</t>
@@ -13837,7 +13851,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="67" s="111">
+    <row customHeight="1" ht="16" r="67" s="121">
       <c r="A67" s="2" t="inlineStr">
         <is>
           <t>Unclassified Accounts</t>
@@ -13928,7 +13942,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="68" s="111" thickBot="1">
+    <row customHeight="1" ht="16" r="68" s="121" thickBot="1">
       <c r="A68" s="33" t="inlineStr">
         <is>
           <t>Wholesale Trade</t>
@@ -14019,7 +14033,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="69" s="111" thickTop="1">
+    <row customHeight="1" ht="17" r="69" s="121" thickTop="1">
       <c r="A69" s="7" t="inlineStr">
         <is>
           <t>Total</t>
@@ -14201,22 +14215,22 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="26" r="74" s="111">
-      <c r="A74" s="119" t="inlineStr">
+    <row customHeight="1" ht="26" r="74" s="121">
+      <c r="A74" s="129" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
-      <c r="B74" s="120" t="n"/>
-      <c r="C74" s="120" t="n"/>
-      <c r="D74" s="120" t="n"/>
-      <c r="E74" s="120" t="n"/>
-      <c r="F74" s="120" t="n"/>
-      <c r="G74" s="120" t="n"/>
-      <c r="H74" s="120" t="n"/>
-      <c r="I74" s="120" t="n"/>
-      <c r="J74" s="120" t="n"/>
-      <c r="K74" s="120" t="n"/>
+      <c r="B74" s="130" t="n"/>
+      <c r="C74" s="130" t="n"/>
+      <c r="D74" s="130" t="n"/>
+      <c r="E74" s="130" t="n"/>
+      <c r="F74" s="130" t="n"/>
+      <c r="G74" s="130" t="n"/>
+      <c r="H74" s="130" t="n"/>
+      <c r="I74" s="130" t="n"/>
+      <c r="J74" s="130" t="n"/>
+      <c r="K74" s="130" t="n"/>
       <c r="L74" s="16" t="n"/>
       <c r="M74" s="16" t="n"/>
       <c r="N74" s="16" t="n"/>
@@ -19506,29 +19520,29 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="117" width="21.6640625"/>
-    <col customWidth="1" max="2" min="2" style="117" width="16.33203125"/>
-    <col bestFit="1" customWidth="1" max="4" min="3" style="117" width="15"/>
-    <col bestFit="1" customWidth="1" max="6" min="5" style="117" width="15.83203125"/>
-    <col bestFit="1" customWidth="1" max="11" min="7" style="117" width="15"/>
-    <col customWidth="1" max="12" min="12" style="117" width="18.1640625"/>
-    <col bestFit="1" customWidth="1" max="13" min="13" style="117" width="15.83203125"/>
-    <col bestFit="1" customWidth="1" max="23" min="14" style="117" width="15"/>
-    <col customWidth="1" max="49" min="24" style="117" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="50" style="117" width="10.83203125"/>
+    <col customWidth="1" max="1" min="1" style="127" width="21.6640625"/>
+    <col customWidth="1" max="2" min="2" style="127" width="16.33203125"/>
+    <col bestFit="1" customWidth="1" max="4" min="3" style="127" width="15"/>
+    <col bestFit="1" customWidth="1" max="6" min="5" style="127" width="15.83203125"/>
+    <col bestFit="1" customWidth="1" max="11" min="7" style="127" width="15"/>
+    <col customWidth="1" max="12" min="12" style="127" width="18.1640625"/>
+    <col bestFit="1" customWidth="1" max="13" min="13" style="127" width="15.83203125"/>
+    <col bestFit="1" customWidth="1" max="23" min="14" style="127" width="15"/>
+    <col customWidth="1" max="51" min="24" style="127" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="52" style="127" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="26" r="1" s="111">
-      <c r="A1" s="116" t="inlineStr">
+    <row customHeight="1" ht="26" r="1" s="121">
+      <c r="A1" s="126" t="inlineStr">
         <is>
           <t>Sales Tax Forecasts</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="3" s="111" thickBot="1">
+    <row customHeight="1" ht="19" r="3" s="121" thickBot="1">
       <c r="B3" s="4" t="n"/>
     </row>
-    <row customHeight="1" ht="19" r="4" s="111" thickBot="1">
+    <row customHeight="1" ht="19" r="4" s="121" thickBot="1">
       <c r="B4" s="4" t="n"/>
       <c r="D4" s="18" t="n"/>
       <c r="E4" s="23" t="inlineStr">
@@ -19542,7 +19556,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="5" s="111">
+    <row customHeight="1" ht="19" r="5" s="121">
       <c r="B5" s="4" t="n"/>
       <c r="D5" s="19" t="inlineStr">
         <is>
@@ -19558,7 +19572,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="6" s="111">
+    <row customHeight="1" ht="19" r="6" s="121">
       <c r="B6" s="4" t="n"/>
       <c r="D6" s="20" t="inlineStr">
         <is>
@@ -19577,7 +19591,7 @@
       <c r="L6" s="32" t="n"/>
       <c r="M6" s="32" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="7" s="111" thickBot="1">
+    <row customHeight="1" ht="17" r="7" s="121" thickBot="1">
       <c r="D7" s="21" t="inlineStr">
         <is>
           <t>FY22</t>
@@ -19592,7 +19606,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="20" r="8" s="111" thickBot="1" thickTop="1">
+    <row customHeight="1" ht="20" r="8" s="121" thickBot="1" thickTop="1">
       <c r="D8" s="22" t="inlineStr">
         <is>
           <t>Total</t>
@@ -19607,12 +19621,12 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="9" s="111">
+    <row customHeight="1" ht="19" r="9" s="121">
       <c r="B9" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="10" s="111"/>
-    <row customHeight="1" ht="26" r="11" s="111">
-      <c r="A11" s="118" t="inlineStr">
+    <row customHeight="1" ht="17" r="10" s="121"/>
+    <row customHeight="1" ht="26" r="11" s="121">
+      <c r="A11" s="128" t="inlineStr">
         <is>
           <t>Moderate Duration Scenario</t>
         </is>
@@ -19636,7 +19650,7 @@
     <row r="13">
       <c r="M13" s="71" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="14" s="111">
+    <row customHeight="1" ht="17" r="14" s="121">
       <c r="M14" s="71" t="n"/>
     </row>
     <row r="15">
@@ -20797,7 +20811,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="28" s="111" thickBot="1">
+    <row customHeight="1" ht="16" r="28" s="121" thickBot="1">
       <c r="A28" s="10" t="inlineStr">
         <is>
           <t>Wholesale</t>
@@ -20888,7 +20902,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="29" s="111" thickTop="1">
+    <row customHeight="1" ht="16" r="29" s="121" thickTop="1">
       <c r="A29" s="7" t="inlineStr">
         <is>
           <t>Total</t>
@@ -21082,7 +21096,7 @@
       <c r="I31" s="73" t="n"/>
       <c r="J31" s="73" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="32" s="111">
+    <row customHeight="1" ht="17" r="32" s="121">
       <c r="A32" s="7" t="n"/>
       <c r="B32" s="73" t="n"/>
       <c r="C32" s="73" t="n"/>
@@ -21094,8 +21108,8 @@
       <c r="I32" s="73" t="n"/>
       <c r="J32" s="73" t="n"/>
     </row>
-    <row customHeight="1" ht="26" r="33" s="111">
-      <c r="A33" s="118" t="inlineStr">
+    <row customHeight="1" ht="26" r="33" s="121">
+      <c r="A33" s="128" t="inlineStr">
         <is>
           <t>Severe Duration Scenario</t>
         </is>
@@ -21119,7 +21133,7 @@
     <row r="35">
       <c r="M35" s="71" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="36" s="111">
+    <row customHeight="1" ht="17" r="36" s="121">
       <c r="M36" s="71" t="n"/>
     </row>
     <row r="37">
@@ -22189,7 +22203,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="49" s="111">
+    <row customHeight="1" ht="16" r="49" s="121">
       <c r="A49" s="7" t="inlineStr">
         <is>
           <t>Total Retail</t>
@@ -22280,7 +22294,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="50" s="111" thickBot="1">
+    <row customHeight="1" ht="16" r="50" s="121" thickBot="1">
       <c r="A50" s="10" t="inlineStr">
         <is>
           <t>Wholesale</t>
@@ -22371,7 +22385,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="51" s="111" thickTop="1">
+    <row customHeight="1" ht="17" r="51" s="121" thickTop="1">
       <c r="A51" s="7" t="inlineStr">
         <is>
           <t>Total</t>
@@ -22553,22 +22567,22 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="26" r="56" s="111">
-      <c r="A56" s="119" t="inlineStr">
+    <row customHeight="1" ht="26" r="56" s="121">
+      <c r="A56" s="129" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
-      <c r="B56" s="120" t="n"/>
-      <c r="C56" s="120" t="n"/>
-      <c r="D56" s="120" t="n"/>
-      <c r="E56" s="120" t="n"/>
-      <c r="F56" s="120" t="n"/>
-      <c r="G56" s="120" t="n"/>
-      <c r="H56" s="120" t="n"/>
-      <c r="I56" s="120" t="n"/>
-      <c r="J56" s="120" t="n"/>
-      <c r="K56" s="120" t="n"/>
+      <c r="B56" s="130" t="n"/>
+      <c r="C56" s="130" t="n"/>
+      <c r="D56" s="130" t="n"/>
+      <c r="E56" s="130" t="n"/>
+      <c r="F56" s="130" t="n"/>
+      <c r="G56" s="130" t="n"/>
+      <c r="H56" s="130" t="n"/>
+      <c r="I56" s="130" t="n"/>
+      <c r="J56" s="130" t="n"/>
+      <c r="K56" s="130" t="n"/>
       <c r="L56" s="16" t="n"/>
       <c r="M56" s="16" t="n"/>
       <c r="N56" s="16" t="n"/>
@@ -25833,27 +25847,27 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="117" width="15.1640625"/>
-    <col customWidth="1" max="2" min="2" style="117" width="16"/>
-    <col bestFit="1" customWidth="1" max="4" min="3" style="117" width="15"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="117" width="14.6640625"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="117" width="15.83203125"/>
-    <col bestFit="1" customWidth="1" max="10" min="7" style="117" width="15"/>
-    <col bestFit="1" customWidth="1" max="12" min="11" style="117" width="16"/>
-    <col bestFit="1" customWidth="1" max="22" min="13" style="117" width="15"/>
-    <col customWidth="1" max="54" min="23" style="117" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="55" style="117" width="10.83203125"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="127" width="15.1640625"/>
+    <col customWidth="1" max="2" min="2" style="127" width="16"/>
+    <col bestFit="1" customWidth="1" max="4" min="3" style="127" width="15"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="127" width="14.6640625"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" style="127" width="15.83203125"/>
+    <col bestFit="1" customWidth="1" max="10" min="7" style="127" width="15"/>
+    <col bestFit="1" customWidth="1" max="12" min="11" style="127" width="16"/>
+    <col bestFit="1" customWidth="1" max="22" min="13" style="127" width="15"/>
+    <col customWidth="1" max="56" min="23" style="127" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="57" style="127" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="26" r="1" s="111">
-      <c r="A1" s="116" t="inlineStr">
+    <row customHeight="1" ht="26" r="1" s="121">
+      <c r="A1" s="126" t="inlineStr">
         <is>
           <t>Realty Transfer Tax (RTT) Forecasts</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="3" s="111" thickBot="1"/>
-    <row customHeight="1" ht="19" r="4" s="111" thickBot="1">
+    <row customHeight="1" ht="17" r="3" s="121" thickBot="1"/>
+    <row customHeight="1" ht="19" r="4" s="121" thickBot="1">
       <c r="B4" s="4" t="n"/>
       <c r="D4" s="18" t="n"/>
       <c r="E4" s="23" t="inlineStr">
@@ -25867,7 +25881,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="5" s="111">
+    <row customHeight="1" ht="19" r="5" s="121">
       <c r="B5" s="4" t="n"/>
       <c r="D5" s="19" t="inlineStr">
         <is>
@@ -25883,7 +25897,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="6" s="111">
+    <row customHeight="1" ht="19" r="6" s="121">
       <c r="B6" s="4" t="n"/>
       <c r="D6" s="20" t="inlineStr">
         <is>
@@ -25899,7 +25913,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="7" s="111" thickBot="1">
+    <row customHeight="1" ht="21" r="7" s="121" thickBot="1">
       <c r="D7" s="21" t="inlineStr">
         <is>
           <t>FY22</t>
@@ -25915,7 +25929,7 @@
       </c>
       <c r="J7" s="32" t="n"/>
     </row>
-    <row customHeight="1" ht="20" r="8" s="111" thickBot="1" thickTop="1">
+    <row customHeight="1" ht="20" r="8" s="121" thickBot="1" thickTop="1">
       <c r="B8" s="11" t="n"/>
       <c r="D8" s="22" t="inlineStr">
         <is>
@@ -25931,14 +25945,14 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="20" r="9" s="111">
+    <row customHeight="1" ht="20" r="9" s="121">
       <c r="B9" s="12" t="n"/>
     </row>
-    <row customHeight="1" ht="19" r="10" s="111">
+    <row customHeight="1" ht="19" r="10" s="121">
       <c r="B10" s="12" t="n"/>
     </row>
-    <row customHeight="1" ht="26" r="11" s="111">
-      <c r="A11" s="118" t="inlineStr">
+    <row customHeight="1" ht="26" r="11" s="121">
+      <c r="A11" s="128" t="inlineStr">
         <is>
           <t>Moderate Scenario</t>
         </is>
@@ -25957,35 +25971,35 @@
       <c r="V11" s="30" t="n"/>
     </row>
     <row r="14">
-      <c r="B14" s="121" t="inlineStr">
+      <c r="B14" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2020</t>
         </is>
       </c>
-      <c r="C14" s="108" t="n"/>
-      <c r="D14" s="108" t="n"/>
-      <c r="E14" s="108" t="n"/>
-      <c r="F14" s="108" t="n"/>
-      <c r="G14" s="108" t="n"/>
-      <c r="H14" s="108" t="n"/>
-      <c r="I14" s="108" t="n"/>
-      <c r="J14" s="109" t="n"/>
-      <c r="K14" s="121" t="inlineStr">
+      <c r="C14" s="118" t="n"/>
+      <c r="D14" s="118" t="n"/>
+      <c r="E14" s="118" t="n"/>
+      <c r="F14" s="118" t="n"/>
+      <c r="G14" s="118" t="n"/>
+      <c r="H14" s="118" t="n"/>
+      <c r="I14" s="118" t="n"/>
+      <c r="J14" s="119" t="n"/>
+      <c r="K14" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2021</t>
         </is>
       </c>
-      <c r="L14" s="108" t="n"/>
-      <c r="M14" s="108" t="n"/>
-      <c r="N14" s="108" t="n"/>
-      <c r="O14" s="108" t="n"/>
-      <c r="P14" s="108" t="n"/>
-      <c r="Q14" s="108" t="n"/>
-      <c r="R14" s="108" t="n"/>
-      <c r="S14" s="108" t="n"/>
-      <c r="T14" s="108" t="n"/>
-      <c r="U14" s="108" t="n"/>
-      <c r="V14" s="109" t="n"/>
+      <c r="L14" s="118" t="n"/>
+      <c r="M14" s="118" t="n"/>
+      <c r="N14" s="118" t="n"/>
+      <c r="O14" s="118" t="n"/>
+      <c r="P14" s="118" t="n"/>
+      <c r="Q14" s="118" t="n"/>
+      <c r="R14" s="118" t="n"/>
+      <c r="S14" s="118" t="n"/>
+      <c r="T14" s="118" t="n"/>
+      <c r="U14" s="118" t="n"/>
+      <c r="V14" s="119" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="n"/>
@@ -26259,8 +26273,8 @@
       <c r="I19" s="73" t="n"/>
       <c r="J19" s="73" t="n"/>
     </row>
-    <row customHeight="1" ht="26" r="20" s="111">
-      <c r="A20" s="118" t="inlineStr">
+    <row customHeight="1" ht="26" r="20" s="121">
+      <c r="A20" s="128" t="inlineStr">
         <is>
           <t>Severe Scenario</t>
         </is>
@@ -26279,35 +26293,35 @@
       <c r="V20" s="30" t="n"/>
     </row>
     <row r="23">
-      <c r="B23" s="121" t="inlineStr">
+      <c r="B23" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2020</t>
         </is>
       </c>
-      <c r="C23" s="108" t="n"/>
-      <c r="D23" s="108" t="n"/>
-      <c r="E23" s="108" t="n"/>
-      <c r="F23" s="108" t="n"/>
-      <c r="G23" s="108" t="n"/>
-      <c r="H23" s="108" t="n"/>
-      <c r="I23" s="108" t="n"/>
-      <c r="J23" s="109" t="n"/>
-      <c r="K23" s="121" t="inlineStr">
+      <c r="C23" s="118" t="n"/>
+      <c r="D23" s="118" t="n"/>
+      <c r="E23" s="118" t="n"/>
+      <c r="F23" s="118" t="n"/>
+      <c r="G23" s="118" t="n"/>
+      <c r="H23" s="118" t="n"/>
+      <c r="I23" s="118" t="n"/>
+      <c r="J23" s="119" t="n"/>
+      <c r="K23" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2021</t>
         </is>
       </c>
-      <c r="L23" s="108" t="n"/>
-      <c r="M23" s="108" t="n"/>
-      <c r="N23" s="108" t="n"/>
-      <c r="O23" s="108" t="n"/>
-      <c r="P23" s="108" t="n"/>
-      <c r="Q23" s="108" t="n"/>
-      <c r="R23" s="108" t="n"/>
-      <c r="S23" s="108" t="n"/>
-      <c r="T23" s="108" t="n"/>
-      <c r="U23" s="108" t="n"/>
-      <c r="V23" s="109" t="n"/>
+      <c r="L23" s="118" t="n"/>
+      <c r="M23" s="118" t="n"/>
+      <c r="N23" s="118" t="n"/>
+      <c r="O23" s="118" t="n"/>
+      <c r="P23" s="118" t="n"/>
+      <c r="Q23" s="118" t="n"/>
+      <c r="R23" s="118" t="n"/>
+      <c r="S23" s="118" t="n"/>
+      <c r="T23" s="118" t="n"/>
+      <c r="U23" s="118" t="n"/>
+      <c r="V23" s="119" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="n"/>
@@ -26557,8 +26571,8 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="26" r="30" s="111">
-      <c r="A30" s="122" t="inlineStr">
+    <row customHeight="1" ht="26" r="30" s="121">
+      <c r="A30" s="132" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
@@ -26856,7 +26870,7 @@
         <v>24017707.77158005</v>
       </c>
     </row>
-    <row customHeight="1" ht="26" r="37" s="111"/>
+    <row customHeight="1" ht="26" r="37" s="121"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A20:J20"/>
@@ -26887,32 +26901,32 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="117" width="21.6640625"/>
-    <col customWidth="1" max="2" min="2" style="117" width="16.33203125"/>
-    <col bestFit="1" customWidth="1" max="6" min="3" style="117" width="16"/>
-    <col bestFit="1" customWidth="1" max="8" min="7" style="117" width="15.1640625"/>
-    <col bestFit="1" customWidth="1" max="10" min="9" style="117" width="16"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="117" width="15.1640625"/>
-    <col customWidth="1" max="12" min="12" style="117" width="18.1640625"/>
-    <col bestFit="1" customWidth="1" max="13" min="13" style="117" width="16"/>
-    <col bestFit="1" customWidth="1" max="14" min="14" style="117" width="15.1640625"/>
-    <col bestFit="1" customWidth="1" max="15" min="15" style="117" width="16"/>
-    <col bestFit="1" customWidth="1" max="23" min="16" style="117" width="15.1640625"/>
-    <col customWidth="1" max="49" min="24" style="117" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="50" style="117" width="10.83203125"/>
+    <col customWidth="1" max="1" min="1" style="127" width="21.6640625"/>
+    <col customWidth="1" max="2" min="2" style="127" width="16.33203125"/>
+    <col bestFit="1" customWidth="1" max="6" min="3" style="127" width="16"/>
+    <col bestFit="1" customWidth="1" max="8" min="7" style="127" width="15.1640625"/>
+    <col bestFit="1" customWidth="1" max="10" min="9" style="127" width="16"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" style="127" width="15.1640625"/>
+    <col customWidth="1" max="12" min="12" style="127" width="18.1640625"/>
+    <col bestFit="1" customWidth="1" max="13" min="13" style="127" width="16"/>
+    <col bestFit="1" customWidth="1" max="14" min="14" style="127" width="15.1640625"/>
+    <col bestFit="1" customWidth="1" max="15" min="15" style="127" width="16"/>
+    <col bestFit="1" customWidth="1" max="23" min="16" style="127" width="15.1640625"/>
+    <col customWidth="1" max="51" min="24" style="127" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="52" style="127" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="26" r="1" s="111">
-      <c r="A1" s="116" t="inlineStr">
+    <row customHeight="1" ht="26" r="1" s="121">
+      <c r="A1" s="126" t="inlineStr">
         <is>
           <t>BIRT Forecasts</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="3" s="111" thickBot="1">
+    <row customHeight="1" ht="19" r="3" s="121" thickBot="1">
       <c r="B3" s="4" t="n"/>
     </row>
-    <row customHeight="1" ht="19" r="4" s="111" thickBot="1">
+    <row customHeight="1" ht="19" r="4" s="121" thickBot="1">
       <c r="B4" s="4" t="n"/>
       <c r="D4" s="18" t="n"/>
       <c r="E4" s="23" t="inlineStr">
@@ -26926,7 +26940,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="5" s="111">
+    <row customHeight="1" ht="19" r="5" s="121">
       <c r="B5" s="4" t="n"/>
       <c r="D5" s="19" t="inlineStr">
         <is>
@@ -26942,7 +26956,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="6" s="111">
+    <row customHeight="1" ht="19" r="6" s="121">
       <c r="B6" s="4" t="n"/>
       <c r="D6" s="20" t="inlineStr">
         <is>
@@ -26961,7 +26975,7 @@
       <c r="L6" s="32" t="n"/>
       <c r="M6" s="32" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="7" s="111" thickBot="1">
+    <row customHeight="1" ht="17" r="7" s="121" thickBot="1">
       <c r="D7" s="21" t="inlineStr">
         <is>
           <t>FY22</t>
@@ -26976,7 +26990,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="20" r="8" s="111" thickBot="1" thickTop="1">
+    <row customHeight="1" ht="20" r="8" s="121" thickBot="1" thickTop="1">
       <c r="D8" s="22" t="inlineStr">
         <is>
           <t>Total</t>
@@ -26991,12 +27005,12 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="9" s="111">
+    <row customHeight="1" ht="19" r="9" s="121">
       <c r="B9" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="10" s="111"/>
-    <row customHeight="1" ht="26" r="11" s="111">
-      <c r="A11" s="118" t="inlineStr">
+    <row customHeight="1" ht="17" r="10" s="121"/>
+    <row customHeight="1" ht="26" r="11" s="121">
+      <c r="A11" s="128" t="inlineStr">
         <is>
           <t>Moderate Duration Scenario</t>
         </is>
@@ -27020,7 +27034,7 @@
     <row r="13">
       <c r="M13" s="71" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="14" s="111">
+    <row customHeight="1" ht="17" r="14" s="121">
       <c r="M14" s="71" t="n"/>
     </row>
     <row r="15">
@@ -28818,7 +28832,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="35" s="111" thickBot="1">
+    <row customHeight="1" ht="17" r="35" s="121" thickBot="1">
       <c r="A35" s="34" t="inlineStr">
         <is>
           <t>Wholesale Trade</t>
@@ -28909,7 +28923,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="36" s="111" thickTop="1">
+    <row customHeight="1" ht="16" r="36" s="121" thickTop="1">
       <c r="A36" s="7" t="inlineStr">
         <is>
           <t>Total</t>
@@ -29103,7 +29117,7 @@
       <c r="I38" s="73" t="n"/>
       <c r="J38" s="73" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="39" s="111">
+    <row customHeight="1" ht="17" r="39" s="121">
       <c r="A39" s="7" t="n"/>
       <c r="B39" s="73" t="n"/>
       <c r="C39" s="73" t="n"/>
@@ -29115,8 +29129,8 @@
       <c r="I39" s="73" t="n"/>
       <c r="J39" s="73" t="n"/>
     </row>
-    <row customHeight="1" ht="26" r="40" s="111">
-      <c r="A40" s="118" t="inlineStr">
+    <row customHeight="1" ht="26" r="40" s="121">
+      <c r="A40" s="128" t="inlineStr">
         <is>
           <t>Severe Duration Scenario</t>
         </is>
@@ -29140,7 +29154,7 @@
     <row r="42">
       <c r="M42" s="71" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="43" s="111">
+    <row customHeight="1" ht="17" r="43" s="121">
       <c r="M43" s="71" t="n"/>
     </row>
     <row r="44">
@@ -30210,7 +30224,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="56" s="111">
+    <row customHeight="1" ht="16" r="56" s="121">
       <c r="A56" s="52" t="inlineStr">
         <is>
           <t>Other Services  **2</t>
@@ -30301,7 +30315,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="57" s="111">
+    <row customHeight="1" ht="16" r="57" s="121">
       <c r="A57" s="52" t="inlineStr">
         <is>
           <t>Professional Services, subtotal</t>
@@ -30392,7 +30406,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="58" s="111">
+    <row customHeight="1" ht="16" r="58" s="121">
       <c r="A58" s="52" t="inlineStr">
         <is>
           <t>Real Estate (including REITS)</t>
@@ -30483,7 +30497,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="59" s="111">
+    <row customHeight="1" ht="16" r="59" s="121">
       <c r="A59" s="52" t="inlineStr">
         <is>
           <t>Restaurants, Bars, and Other Food Services</t>
@@ -30574,7 +30588,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="60" s="111">
+    <row customHeight="1" ht="16" r="60" s="121">
       <c r="A60" s="52" t="inlineStr">
         <is>
           <t>Retail Trade</t>
@@ -30665,7 +30679,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="61" s="111">
+    <row customHeight="1" ht="16" r="61" s="121">
       <c r="A61" s="52" t="inlineStr">
         <is>
           <t>Sports</t>
@@ -30756,7 +30770,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="62" s="111">
+    <row customHeight="1" ht="16" r="62" s="121">
       <c r="A62" s="52" t="inlineStr">
         <is>
           <t>Transportation and Storage</t>
@@ -30847,7 +30861,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="63" s="111">
+    <row customHeight="1" ht="16" r="63" s="121">
       <c r="A63" s="52" t="inlineStr">
         <is>
           <t>Unclassified</t>
@@ -30938,7 +30952,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="64" s="111" thickBot="1">
+    <row customHeight="1" ht="16" r="64" s="121" thickBot="1">
       <c r="A64" s="34" t="inlineStr">
         <is>
           <t>Wholesale Trade</t>
@@ -31029,7 +31043,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="65" s="111" thickTop="1">
+    <row customHeight="1" ht="17" r="65" s="121" thickTop="1">
       <c r="A65" s="7" t="inlineStr">
         <is>
           <t>Total</t>
@@ -31211,22 +31225,22 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="26" r="70" s="111">
-      <c r="A70" s="119" t="inlineStr">
+    <row customHeight="1" ht="26" r="70" s="121">
+      <c r="A70" s="129" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
-      <c r="B70" s="120" t="n"/>
-      <c r="C70" s="120" t="n"/>
-      <c r="D70" s="120" t="n"/>
-      <c r="E70" s="120" t="n"/>
-      <c r="F70" s="120" t="n"/>
-      <c r="G70" s="120" t="n"/>
-      <c r="H70" s="120" t="n"/>
-      <c r="I70" s="120" t="n"/>
-      <c r="J70" s="120" t="n"/>
-      <c r="K70" s="120" t="n"/>
+      <c r="B70" s="130" t="n"/>
+      <c r="C70" s="130" t="n"/>
+      <c r="D70" s="130" t="n"/>
+      <c r="E70" s="130" t="n"/>
+      <c r="F70" s="130" t="n"/>
+      <c r="G70" s="130" t="n"/>
+      <c r="H70" s="130" t="n"/>
+      <c r="I70" s="130" t="n"/>
+      <c r="J70" s="130" t="n"/>
+      <c r="K70" s="130" t="n"/>
       <c r="L70" s="16" t="n"/>
       <c r="M70" s="16" t="n"/>
       <c r="N70" s="16" t="n"/>
@@ -36066,24 +36080,24 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="117" width="15.1640625"/>
-    <col customWidth="1" max="2" min="2" style="117" width="16"/>
-    <col bestFit="1" customWidth="1" max="10" min="3" style="117" width="15"/>
-    <col bestFit="1" customWidth="1" max="12" min="11" style="117" width="16"/>
-    <col bestFit="1" customWidth="1" max="22" min="13" style="117" width="15"/>
-    <col customWidth="1" max="54" min="23" style="117" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="55" style="117" width="10.83203125"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="127" width="15.1640625"/>
+    <col customWidth="1" max="2" min="2" style="127" width="16"/>
+    <col bestFit="1" customWidth="1" max="10" min="3" style="127" width="15"/>
+    <col bestFit="1" customWidth="1" max="12" min="11" style="127" width="16"/>
+    <col bestFit="1" customWidth="1" max="22" min="13" style="127" width="15"/>
+    <col customWidth="1" max="56" min="23" style="127" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="57" style="127" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="26" r="1" s="111">
-      <c r="A1" s="116" t="inlineStr">
+    <row customHeight="1" ht="26" r="1" s="121">
+      <c r="A1" s="126" t="inlineStr">
         <is>
           <t>Soda Tax Forecasts</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="3" s="111" thickBot="1"/>
-    <row customHeight="1" ht="19" r="4" s="111" thickBot="1">
+    <row customHeight="1" ht="17" r="3" s="121" thickBot="1"/>
+    <row customHeight="1" ht="19" r="4" s="121" thickBot="1">
       <c r="B4" s="4" t="n"/>
       <c r="D4" s="18" t="n"/>
       <c r="E4" s="23" t="inlineStr">
@@ -36097,7 +36111,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="5" s="111">
+    <row customHeight="1" ht="19" r="5" s="121">
       <c r="B5" s="4" t="n"/>
       <c r="D5" s="19" t="inlineStr">
         <is>
@@ -36113,7 +36127,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="6" s="111">
+    <row customHeight="1" ht="19" r="6" s="121">
       <c r="B6" s="4" t="n"/>
       <c r="D6" s="20" t="inlineStr">
         <is>
@@ -36129,7 +36143,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="21" r="7" s="111" thickBot="1">
+    <row customHeight="1" ht="21" r="7" s="121" thickBot="1">
       <c r="D7" s="21" t="inlineStr">
         <is>
           <t>FY22</t>
@@ -36145,7 +36159,7 @@
       </c>
       <c r="J7" s="32" t="n"/>
     </row>
-    <row customHeight="1" ht="20" r="8" s="111" thickBot="1" thickTop="1">
+    <row customHeight="1" ht="20" r="8" s="121" thickBot="1" thickTop="1">
       <c r="B8" s="11" t="n"/>
       <c r="D8" s="22" t="inlineStr">
         <is>
@@ -36161,11 +36175,11 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="9" s="111">
+    <row customHeight="1" ht="19" r="9" s="121">
       <c r="B9" s="4" t="n"/>
     </row>
-    <row customHeight="1" ht="26" r="11" s="111">
-      <c r="A11" s="118" t="inlineStr">
+    <row customHeight="1" ht="26" r="11" s="121">
+      <c r="A11" s="128" t="inlineStr">
         <is>
           <t>Moderate Scenario</t>
         </is>
@@ -36184,35 +36198,35 @@
       <c r="V11" s="30" t="n"/>
     </row>
     <row r="14">
-      <c r="B14" s="121" t="inlineStr">
+      <c r="B14" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2020</t>
         </is>
       </c>
-      <c r="C14" s="108" t="n"/>
-      <c r="D14" s="108" t="n"/>
-      <c r="E14" s="108" t="n"/>
-      <c r="F14" s="108" t="n"/>
-      <c r="G14" s="108" t="n"/>
-      <c r="H14" s="108" t="n"/>
-      <c r="I14" s="108" t="n"/>
-      <c r="J14" s="109" t="n"/>
-      <c r="K14" s="121" t="inlineStr">
+      <c r="C14" s="118" t="n"/>
+      <c r="D14" s="118" t="n"/>
+      <c r="E14" s="118" t="n"/>
+      <c r="F14" s="118" t="n"/>
+      <c r="G14" s="118" t="n"/>
+      <c r="H14" s="118" t="n"/>
+      <c r="I14" s="118" t="n"/>
+      <c r="J14" s="119" t="n"/>
+      <c r="K14" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2021</t>
         </is>
       </c>
-      <c r="L14" s="108" t="n"/>
-      <c r="M14" s="108" t="n"/>
-      <c r="N14" s="108" t="n"/>
-      <c r="O14" s="108" t="n"/>
-      <c r="P14" s="108" t="n"/>
-      <c r="Q14" s="108" t="n"/>
-      <c r="R14" s="108" t="n"/>
-      <c r="S14" s="108" t="n"/>
-      <c r="T14" s="108" t="n"/>
-      <c r="U14" s="108" t="n"/>
-      <c r="V14" s="109" t="n"/>
+      <c r="L14" s="118" t="n"/>
+      <c r="M14" s="118" t="n"/>
+      <c r="N14" s="118" t="n"/>
+      <c r="O14" s="118" t="n"/>
+      <c r="P14" s="118" t="n"/>
+      <c r="Q14" s="118" t="n"/>
+      <c r="R14" s="118" t="n"/>
+      <c r="S14" s="118" t="n"/>
+      <c r="T14" s="118" t="n"/>
+      <c r="U14" s="118" t="n"/>
+      <c r="V14" s="119" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="n"/>
@@ -36486,8 +36500,8 @@
       <c r="I19" s="73" t="n"/>
       <c r="J19" s="73" t="n"/>
     </row>
-    <row customHeight="1" ht="26" r="20" s="111">
-      <c r="A20" s="118" t="inlineStr">
+    <row customHeight="1" ht="26" r="20" s="121">
+      <c r="A20" s="128" t="inlineStr">
         <is>
           <t>Severe Scenario</t>
         </is>
@@ -36506,35 +36520,35 @@
       <c r="V20" s="30" t="n"/>
     </row>
     <row r="23">
-      <c r="B23" s="121" t="inlineStr">
+      <c r="B23" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2020</t>
         </is>
       </c>
-      <c r="C23" s="108" t="n"/>
-      <c r="D23" s="108" t="n"/>
-      <c r="E23" s="108" t="n"/>
-      <c r="F23" s="108" t="n"/>
-      <c r="G23" s="108" t="n"/>
-      <c r="H23" s="108" t="n"/>
-      <c r="I23" s="108" t="n"/>
-      <c r="J23" s="109" t="n"/>
-      <c r="K23" s="121" t="inlineStr">
+      <c r="C23" s="118" t="n"/>
+      <c r="D23" s="118" t="n"/>
+      <c r="E23" s="118" t="n"/>
+      <c r="F23" s="118" t="n"/>
+      <c r="G23" s="118" t="n"/>
+      <c r="H23" s="118" t="n"/>
+      <c r="I23" s="118" t="n"/>
+      <c r="J23" s="119" t="n"/>
+      <c r="K23" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2021</t>
         </is>
       </c>
-      <c r="L23" s="108" t="n"/>
-      <c r="M23" s="108" t="n"/>
-      <c r="N23" s="108" t="n"/>
-      <c r="O23" s="108" t="n"/>
-      <c r="P23" s="108" t="n"/>
-      <c r="Q23" s="108" t="n"/>
-      <c r="R23" s="108" t="n"/>
-      <c r="S23" s="108" t="n"/>
-      <c r="T23" s="108" t="n"/>
-      <c r="U23" s="108" t="n"/>
-      <c r="V23" s="109" t="n"/>
+      <c r="L23" s="118" t="n"/>
+      <c r="M23" s="118" t="n"/>
+      <c r="N23" s="118" t="n"/>
+      <c r="O23" s="118" t="n"/>
+      <c r="P23" s="118" t="n"/>
+      <c r="Q23" s="118" t="n"/>
+      <c r="R23" s="118" t="n"/>
+      <c r="S23" s="118" t="n"/>
+      <c r="T23" s="118" t="n"/>
+      <c r="U23" s="118" t="n"/>
+      <c r="V23" s="119" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="n"/>
@@ -36784,8 +36798,8 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="26" r="30" s="111">
-      <c r="A30" s="122" t="inlineStr">
+    <row customHeight="1" ht="26" r="30" s="121">
+      <c r="A30" s="132" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
@@ -37113,23 +37127,23 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="117" width="15.1640625"/>
-    <col bestFit="1" customWidth="1" max="4" min="2" style="117" width="14"/>
-    <col bestFit="1" customWidth="1" max="6" min="5" style="117" width="14.6640625"/>
-    <col bestFit="1" customWidth="1" max="22" min="7" style="117" width="14"/>
-    <col customWidth="1" max="54" min="23" style="117" width="10.83203125"/>
-    <col customWidth="1" max="16384" min="55" style="117" width="10.83203125"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="127" width="15.1640625"/>
+    <col bestFit="1" customWidth="1" max="4" min="2" style="127" width="14"/>
+    <col bestFit="1" customWidth="1" max="6" min="5" style="127" width="14.6640625"/>
+    <col bestFit="1" customWidth="1" max="22" min="7" style="127" width="14"/>
+    <col customWidth="1" max="56" min="23" style="127" width="10.83203125"/>
+    <col customWidth="1" max="16384" min="57" style="127" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="26" r="1" s="111">
-      <c r="A1" s="116" t="inlineStr">
+    <row customHeight="1" ht="26" r="1" s="121">
+      <c r="A1" s="126" t="inlineStr">
         <is>
           <t>Parking Tax Forecasts</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="3" s="111" thickBot="1"/>
-    <row customHeight="1" ht="21" r="4" s="111" thickBot="1">
+    <row customHeight="1" ht="19" r="3" s="121" thickBot="1"/>
+    <row customHeight="1" ht="21" r="4" s="121" thickBot="1">
       <c r="D4" s="18" t="n"/>
       <c r="E4" s="23" t="inlineStr">
         <is>
@@ -37142,7 +37156,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="20" r="5" s="111">
+    <row customHeight="1" ht="20" r="5" s="121">
       <c r="D5" s="19" t="inlineStr">
         <is>
           <t>FY20</t>
@@ -37157,7 +37171,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="20" r="6" s="111">
+    <row customHeight="1" ht="20" r="6" s="121">
       <c r="D6" s="20" t="inlineStr">
         <is>
           <t>FY21</t>
@@ -37172,7 +37186,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="7" s="111" thickBot="1">
+    <row customHeight="1" ht="19" r="7" s="121" thickBot="1">
       <c r="D7" s="21" t="inlineStr">
         <is>
           <t>FY22</t>
@@ -37187,7 +37201,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="19" r="8" s="111" thickBot="1" thickTop="1">
+    <row customHeight="1" ht="19" r="8" s="121" thickBot="1" thickTop="1">
       <c r="D8" s="22" t="inlineStr">
         <is>
           <t>Total</t>
@@ -37202,12 +37216,12 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="20" r="9" s="111">
+    <row customHeight="1" ht="20" r="9" s="121">
       <c r="D9" s="17" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="10" s="111"/>
-    <row customHeight="1" ht="26" r="11" s="111">
-      <c r="A11" s="118" t="inlineStr">
+    <row customHeight="1" ht="17" r="10" s="121"/>
+    <row customHeight="1" ht="26" r="11" s="121">
+      <c r="A11" s="128" t="inlineStr">
         <is>
           <t>Moderate Scenario</t>
         </is>
@@ -37225,36 +37239,36 @@
       <c r="U11" s="30" t="n"/>
       <c r="V11" s="30" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="14" s="111">
-      <c r="B14" s="121" t="inlineStr">
+    <row customHeight="1" ht="17" r="14" s="121">
+      <c r="B14" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2020</t>
         </is>
       </c>
-      <c r="C14" s="108" t="n"/>
-      <c r="D14" s="108" t="n"/>
-      <c r="E14" s="108" t="n"/>
-      <c r="F14" s="108" t="n"/>
-      <c r="G14" s="108" t="n"/>
-      <c r="H14" s="108" t="n"/>
-      <c r="I14" s="108" t="n"/>
-      <c r="J14" s="109" t="n"/>
-      <c r="K14" s="121" t="inlineStr">
+      <c r="C14" s="118" t="n"/>
+      <c r="D14" s="118" t="n"/>
+      <c r="E14" s="118" t="n"/>
+      <c r="F14" s="118" t="n"/>
+      <c r="G14" s="118" t="n"/>
+      <c r="H14" s="118" t="n"/>
+      <c r="I14" s="118" t="n"/>
+      <c r="J14" s="119" t="n"/>
+      <c r="K14" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2021</t>
         </is>
       </c>
-      <c r="L14" s="108" t="n"/>
-      <c r="M14" s="108" t="n"/>
-      <c r="N14" s="108" t="n"/>
-      <c r="O14" s="108" t="n"/>
-      <c r="P14" s="108" t="n"/>
-      <c r="Q14" s="108" t="n"/>
-      <c r="R14" s="108" t="n"/>
-      <c r="S14" s="108" t="n"/>
-      <c r="T14" s="108" t="n"/>
-      <c r="U14" s="108" t="n"/>
-      <c r="V14" s="109" t="n"/>
+      <c r="L14" s="118" t="n"/>
+      <c r="M14" s="118" t="n"/>
+      <c r="N14" s="118" t="n"/>
+      <c r="O14" s="118" t="n"/>
+      <c r="P14" s="118" t="n"/>
+      <c r="Q14" s="118" t="n"/>
+      <c r="R14" s="118" t="n"/>
+      <c r="S14" s="118" t="n"/>
+      <c r="T14" s="118" t="n"/>
+      <c r="U14" s="118" t="n"/>
+      <c r="V14" s="119" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="5" t="n"/>
@@ -37516,7 +37530,7 @@
       <c r="I18" s="73" t="n"/>
       <c r="J18" s="73" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="19" s="111">
+    <row customHeight="1" ht="17" r="19" s="121">
       <c r="A19" s="7" t="n"/>
       <c r="B19" s="73" t="n"/>
       <c r="C19" s="73" t="n"/>
@@ -37528,8 +37542,8 @@
       <c r="I19" s="73" t="n"/>
       <c r="J19" s="73" t="n"/>
     </row>
-    <row customHeight="1" ht="26" r="20" s="111">
-      <c r="A20" s="118" t="inlineStr">
+    <row customHeight="1" ht="26" r="20" s="121">
+      <c r="A20" s="128" t="inlineStr">
         <is>
           <t>Severe Scenario</t>
         </is>
@@ -37547,36 +37561,36 @@
       <c r="U20" s="30" t="n"/>
       <c r="V20" s="30" t="n"/>
     </row>
-    <row customHeight="1" ht="17" r="23" s="111">
-      <c r="B23" s="121" t="inlineStr">
+    <row customHeight="1" ht="17" r="23" s="121">
+      <c r="B23" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2020</t>
         </is>
       </c>
-      <c r="C23" s="108" t="n"/>
-      <c r="D23" s="108" t="n"/>
-      <c r="E23" s="108" t="n"/>
-      <c r="F23" s="108" t="n"/>
-      <c r="G23" s="108" t="n"/>
-      <c r="H23" s="108" t="n"/>
-      <c r="I23" s="108" t="n"/>
-      <c r="J23" s="109" t="n"/>
-      <c r="K23" s="121" t="inlineStr">
+      <c r="C23" s="118" t="n"/>
+      <c r="D23" s="118" t="n"/>
+      <c r="E23" s="118" t="n"/>
+      <c r="F23" s="118" t="n"/>
+      <c r="G23" s="118" t="n"/>
+      <c r="H23" s="118" t="n"/>
+      <c r="I23" s="118" t="n"/>
+      <c r="J23" s="119" t="n"/>
+      <c r="K23" s="131" t="inlineStr">
         <is>
           <t>Calendar Year 2021</t>
         </is>
       </c>
-      <c r="L23" s="108" t="n"/>
-      <c r="M23" s="108" t="n"/>
-      <c r="N23" s="108" t="n"/>
-      <c r="O23" s="108" t="n"/>
-      <c r="P23" s="108" t="n"/>
-      <c r="Q23" s="108" t="n"/>
-      <c r="R23" s="108" t="n"/>
-      <c r="S23" s="108" t="n"/>
-      <c r="T23" s="108" t="n"/>
-      <c r="U23" s="108" t="n"/>
-      <c r="V23" s="109" t="n"/>
+      <c r="L23" s="118" t="n"/>
+      <c r="M23" s="118" t="n"/>
+      <c r="N23" s="118" t="n"/>
+      <c r="O23" s="118" t="n"/>
+      <c r="P23" s="118" t="n"/>
+      <c r="Q23" s="118" t="n"/>
+      <c r="R23" s="118" t="n"/>
+      <c r="S23" s="118" t="n"/>
+      <c r="T23" s="118" t="n"/>
+      <c r="U23" s="118" t="n"/>
+      <c r="V23" s="119" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="5" t="n"/>
@@ -37826,8 +37840,8 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="26" r="30" s="111">
-      <c r="A30" s="122" t="inlineStr">
+    <row customHeight="1" ht="26" r="30" s="121">
+      <c r="A30" s="132" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
@@ -38125,17 +38139,17 @@
         <v>8417071.608904393</v>
       </c>
     </row>
-    <row customHeight="1" ht="26" r="37" s="111"/>
+    <row customHeight="1" ht="26" r="37" s="121"/>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="K14:V14"/>
-    <mergeCell ref="K23:V23"/>
-    <mergeCell ref="B23:J23"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A20:J20"/>
     <mergeCell ref="A30:J30"/>
     <mergeCell ref="B14:J14"/>
+    <mergeCell ref="K14:V14"/>
+    <mergeCell ref="K23:V23"/>
+    <mergeCell ref="B23:J23"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>